<commit_message>
クラス名等変更 editPairing -> editCompareInfo
</commit_message>
<xml_diff>
--- a/xyz.hotchpotch.hogandiff/messages.properties管理.xlsx
+++ b/xyz.hotchpotch.hogandiff/messages.properties管理.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ya_na\git\hogandiff4\xyz.hotchpotch.hogandiff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009FE7A4-142F-4DBE-8C6B-D190CF27E0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2D98B-1195-47CC-B06C-2B4A48D4E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1876,10 +1876,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>fx.EditPairingPane.010</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>組み合わせ編集</t>
     <rPh sb="0" eb="1">
       <t>ク</t>
@@ -1898,6 +1894,10 @@
   </si>
   <si>
     <t>组合编辑</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fx.EditCompareInfoPane.010</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3133,28 +3133,28 @@
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>496</v>
-      </c>
       <c r="G31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>fx.EditPairingPane.010=組み合わせ編集</v>
+        <v>fx.EditCompareInfoPane.010=組み合わせ編集</v>
       </c>
       <c r="H31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>fx.EditPairingPane.010=Edit Pairing</v>
+        <v>fx.EditCompareInfoPane.010=Edit Pairing</v>
       </c>
       <c r="I31" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>fx.EditPairingPane.010=组合编辑</v>
+        <v>fx.EditCompareInfoPane.010=组合编辑</v>
       </c>
     </row>
     <row r="32" spans="2:9">

</xml_diff>

<commit_message>
名前変更 CompareInfo -> Comparison
</commit_message>
<xml_diff>
--- a/xyz.hotchpotch.hogandiff/messages.properties管理.xlsx
+++ b/xyz.hotchpotch.hogandiff/messages.properties管理.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ya_na\git\hogandiff4\xyz.hotchpotch.hogandiff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2D98B-1195-47CC-B06C-2B4A48D4E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC57292-6BAC-426F-BE5B-F76E6669D042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1897,7 +1897,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>fx.EditCompareInfoPane.010</t>
+    <t>fx.EditComparisonPane.010</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3146,15 +3146,15 @@
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>fx.EditCompareInfoPane.010=組み合わせ編集</v>
+        <v>fx.EditComparisonPane.010=組み合わせ編集</v>
       </c>
       <c r="H31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>fx.EditCompareInfoPane.010=Edit Pairing</v>
+        <v>fx.EditComparisonPane.010=Edit Pairing</v>
       </c>
       <c r="I31" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>fx.EditCompareInfoPane.010=组合编辑</v>
+        <v>fx.EditComparisonPane.010=组合编辑</v>
       </c>
     </row>
     <row r="32" spans="2:9">

</xml_diff>